<commit_message>
version 2 etapa 1
</commit_message>
<xml_diff>
--- a/doc/bodega_cueros.xlsx
+++ b/doc/bodega_cueros.xlsx
@@ -5,15 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Langriss\Desktop\Full Stack Python\Modulo 4 BASES DE DATOS\Ejercicio Individual 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Langriss\Desktop\Full Stack Python\Modulo 4 BASES DE DATOS\Ejercicio Individual 1\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8820" windowHeight="2565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8820" windowHeight="2565" tabRatio="594"/>
   </bookViews>
   <sheets>
-    <sheet name="Compras" sheetId="1" r:id="rId1"/>
-    <sheet name="Resumen" sheetId="2" r:id="rId2"/>
+    <sheet name="Materia Prima" sheetId="1" r:id="rId1"/>
+    <sheet name="Productos Existencia" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId3"/>
+    <sheet name="Resumen" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="51">
   <si>
     <t>Orden de compra</t>
   </si>
@@ -69,21 +71,127 @@
     <t>Stock Grados</t>
   </si>
   <si>
-    <t>Valor Actual Activos</t>
+    <t>Costo total x grado</t>
   </si>
   <si>
-    <t>Costo total x grado</t>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>BC4</t>
+  </si>
+  <si>
+    <t>AX50</t>
+  </si>
+  <si>
+    <t>Billetera</t>
+  </si>
+  <si>
+    <t>Cartera</t>
+  </si>
+  <si>
+    <t>HH54</t>
+  </si>
+  <si>
+    <t>HT567</t>
+  </si>
+  <si>
+    <t>Guantes</t>
+  </si>
+  <si>
+    <t>IJU</t>
+  </si>
+  <si>
+    <t>Botas</t>
+  </si>
+  <si>
+    <t>XXS67</t>
+  </si>
+  <si>
+    <t>OPIH6</t>
+  </si>
+  <si>
+    <t>Grado de Cuero</t>
+  </si>
+  <si>
+    <t>Activos - Materia Prima</t>
+  </si>
+  <si>
+    <t>Activos - Productos</t>
+  </si>
+  <si>
+    <t>alex</t>
+  </si>
+  <si>
+    <t>monroo</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Precio Unitario</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Cartera BC4</t>
+  </si>
+  <si>
+    <t>Guantes IJU</t>
+  </si>
+  <si>
+    <t>Billetera HH54</t>
+  </si>
+  <si>
+    <t>Anabella</t>
+  </si>
+  <si>
+    <t>Casic</t>
+  </si>
+  <si>
+    <t>Carmen</t>
+  </si>
+  <si>
+    <t>Alix</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Lee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-340A]\ * #,##0_-;\-[$$-340A]\ * #,##0_-;_-[$$-340A]\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-[$$-340A]\ * #,##0_-;\-[$$-340A]\ * #,##0_-;_-[$$-340A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +246,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +268,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -176,16 +310,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -194,16 +343,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -256,7 +436,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Grado 2 - Cartera </a:t>
+              <a:t>Grado 0,4 - Cartera </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -326,7 +506,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Compras!$B$4,Compras!$B$12,Compras!$B$20)</c:f>
+              <c:f>('Materia Prima'!$B$4,'Materia Prima'!$B$12,'Materia Prima'!$B$20)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="3"/>
@@ -344,7 +524,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Compras!$H$5,Compras!$H$13,Compras!$H$21)</c:f>
+              <c:f>('Materia Prima'!$H$5,'Materia Prima'!$H$13,'Materia Prima'!$H$21)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -570,7 +750,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Grado 2 - Guantes </a:t>
+              <a:t>Grado 0,2 - Guantes </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -640,7 +820,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Compras!$B$4,Compras!$B$12,Compras!$B$20)</c:f>
+              <c:f>('Materia Prima'!$B$4,'Materia Prima'!$B$12,'Materia Prima'!$B$20)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="3"/>
@@ -658,7 +838,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Compras!$H$6,Compras!$H$14,Compras!$H$22)</c:f>
+              <c:f>('Materia Prima'!$H$6,'Materia Prima'!$H$14,'Materia Prima'!$H$22)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -884,7 +1064,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Grado 2 - Billetera </a:t>
+              <a:t>Grado 0,1 - Billetera </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -954,7 +1134,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Compras!$B$4,Compras!$B$12,Compras!$B$20)</c:f>
+              <c:f>('Materia Prima'!$B$4,'Materia Prima'!$B$12,'Materia Prima'!$B$20)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="3"/>
@@ -972,7 +1152,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Compras!$H$4,Compras!$H$12,Compras!$H$20)</c:f>
+              <c:f>('Materia Prima'!$H$4,'Materia Prima'!$H$12,'Materia Prima'!$H$20)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1198,7 +1378,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Grado 2 - Botas  </a:t>
+              <a:t>Grado 0,5 - Botas  </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1268,7 +1448,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Compras!$B$4,Compras!$B$12,Compras!$B$20)</c:f>
+              <c:f>('Materia Prima'!$B$4,'Materia Prima'!$B$12,'Materia Prima'!$B$20)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1286,7 +1466,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Compras!$H$7,Compras!$H$15,Compras!$H$23)</c:f>
+              <c:f>('Materia Prima'!$H$7,'Materia Prima'!$H$15,'Materia Prima'!$H$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3838,16 +4018,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3870,16 +4050,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>738187</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>695324</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>754855</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3903,15 +4083,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>752475</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>159544</xdr:rowOff>
+      <xdr:rowOff>183356</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>140493</xdr:rowOff>
+      <xdr:rowOff>164305</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3934,16 +4114,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>130969</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>178593</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>207168</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>159542</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4234,13 +4414,14 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
@@ -4248,442 +4429,442 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5"/>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>134123443</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>44054</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>100</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>300</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <f>F4*G4</f>
         <v>30000</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>50</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>400</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f t="shared" ref="H5:H7" si="0">F5*G5</f>
         <v>20000</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.4</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>60</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>500</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>90</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>790</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>71100</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="3">
-        <f>SUM(Compras!F4:F7)</f>
+      <c r="F8" s="2">
+        <f>SUM('Materia Prima'!F4:F7)</f>
         <v>300</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="3">
-        <f>SUM(Compras!H4:H7)</f>
+      <c r="F9" s="2">
+        <f>SUM('Materia Prima'!H4:H7)</f>
         <v>151100</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>15</v>
+      <c r="H11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>134123443</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>44115</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>0.1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>100</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>350</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <f>F12*G12</f>
         <v>35000</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>2</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>0.2</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>10</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>400</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <f t="shared" ref="H13:H15" si="1">F13*G13</f>
         <v>4000</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>3</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>0.4</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>60</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>500</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <f t="shared" si="1"/>
         <v>30000</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>4</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>0.5</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>100</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>600</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <f t="shared" si="1"/>
         <v>60000</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="3">
-        <f>SUM(Compras!F12:F15)</f>
+      <c r="F16" s="2">
+        <f>SUM('Materia Prima'!F12:F15)</f>
         <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="3">
-        <f>SUM(Compras!H12:H15)</f>
+      <c r="F17" s="2">
+        <f>SUM('Materia Prima'!H12:H15)</f>
         <v>129000</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>15</v>
+      <c r="H19" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>134123443</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>44146</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>0.1</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>100</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>700</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <f>F20*G20</f>
         <v>70000</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
         <v>2</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>0.2</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>50</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>900</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <f t="shared" ref="H21:H23" si="2">F21*G21</f>
         <v>45000</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
         <v>3</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>0.4</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>60</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>1100</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <f t="shared" si="2"/>
         <v>66000</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
         <v>4</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>0.5</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>200</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>1250</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <f t="shared" si="2"/>
         <v>250000</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="3">
-        <f>SUM(Compras!F20:F23)</f>
+      <c r="F24" s="2">
+        <f>SUM('Materia Prima'!F20:F23)</f>
         <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="3">
-        <f>SUM(Compras!H20:H23)</f>
+      <c r="F25" s="2">
+        <f>SUM('Materia Prima'!H20:H23)</f>
         <v>431000</v>
       </c>
     </row>
@@ -4698,11 +4879,1322 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>23000</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3">
+        <v>10000</v>
+      </c>
+      <c r="K3">
+        <v>0.2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3">
+        <v>20000</v>
+      </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>23000</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <v>10000</v>
+      </c>
+      <c r="K4">
+        <v>0.2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4">
+        <v>20000</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>23000</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <v>10000</v>
+      </c>
+      <c r="K5">
+        <v>0.2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5">
+        <v>20000</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>23000</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>10000</v>
+      </c>
+      <c r="K6">
+        <v>0.2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6">
+        <v>20000</v>
+      </c>
+      <c r="P6">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>23000</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7">
+        <v>10000</v>
+      </c>
+      <c r="K7">
+        <v>0.2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7">
+        <v>20000</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>23000</v>
+      </c>
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8">
+        <v>10000</v>
+      </c>
+      <c r="K8">
+        <v>0.2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8">
+        <v>20000</v>
+      </c>
+      <c r="P8">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>15000</v>
+      </c>
+      <c r="F9">
+        <v>0.1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9">
+        <v>10000</v>
+      </c>
+      <c r="K9">
+        <v>0.2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9">
+        <v>20000</v>
+      </c>
+      <c r="P9">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>15000</v>
+      </c>
+      <c r="F10">
+        <v>0.1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <v>10000</v>
+      </c>
+      <c r="K10">
+        <v>0.2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10">
+        <v>20000</v>
+      </c>
+      <c r="P10">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>15000</v>
+      </c>
+      <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11">
+        <v>25000</v>
+      </c>
+      <c r="P11">
+        <v>0.5</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>26</v>
+      </c>
+      <c r="R11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>15000</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12">
+        <v>25000</v>
+      </c>
+      <c r="P12">
+        <v>0.5</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>26</v>
+      </c>
+      <c r="R12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>15000</v>
+      </c>
+      <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13">
+        <v>25000</v>
+      </c>
+      <c r="P13">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>15000</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14">
+        <v>25000</v>
+      </c>
+      <c r="P14">
+        <v>0.5</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>15000</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15">
+        <v>25000</v>
+      </c>
+      <c r="P15">
+        <v>0.5</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>26</v>
+      </c>
+      <c r="R15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>15000</v>
+      </c>
+      <c r="F16">
+        <v>0.1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16">
+        <v>25000</v>
+      </c>
+      <c r="P16">
+        <v>0.5</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>26</v>
+      </c>
+      <c r="R16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S16">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="17" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0.1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17">
+        <v>25000</v>
+      </c>
+      <c r="P17">
+        <v>0.5</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>26</v>
+      </c>
+      <c r="R17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="18" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18">
+        <v>25000</v>
+      </c>
+      <c r="P18">
+        <v>0.5</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>26</v>
+      </c>
+      <c r="R18" t="s">
+        <v>28</v>
+      </c>
+      <c r="S18">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="19" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>0.5</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>26</v>
+      </c>
+      <c r="R19" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="20" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>0.5</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>26</v>
+      </c>
+      <c r="R20" t="s">
+        <v>28</v>
+      </c>
+      <c r="S20">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="21" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>0.5</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>26</v>
+      </c>
+      <c r="R21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="22" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>0.5</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>26</v>
+      </c>
+      <c r="R22" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="23" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>0.5</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>26</v>
+      </c>
+      <c r="R23" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="26" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J27" s="11"/>
+      <c r="N27" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="M1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="8" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>23000</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="21">
+        <f>SUM(G4:G6)</f>
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>23000</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="21">
+        <f>SUM(G9:G11)</f>
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>23000</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="21">
+        <f>SUM(G13:G15)</f>
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>23000</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3">
+        <v>44114</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="21">
+        <f>SUM(G18:G20)</f>
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="C1:J9"/>
+  <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="K1" sqref="C1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4710,90 +6202,112 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="3:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="10">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="3:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="7">
         <v>0.1</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>0.2</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="7">
         <v>0.4</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <v>0.5</v>
       </c>
-      <c r="G3" s="9">
-        <f>SUM(Compras!F9,Compras!F17,Compras!F25)</f>
+      <c r="G3" s="10">
+        <f>SUM('Materia Prima'!F9,'Materia Prima'!F17,'Materia Prima'!F25)</f>
         <v>711100</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="3">
-        <f>SUM(Compras!F4,Compras!F12,Compras!F20)</f>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="15">
+        <f>SUM('Productos Existencia'!D3:D33,'Productos Existencia'!I3:I33,'Productos Existencia'!N3:N33,'Productos Existencia'!S3:S33)</f>
+        <v>1808000</v>
+      </c>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <f>SUM('Materia Prima'!F4,'Materia Prima'!F12,'Materia Prima'!F20)</f>
         <v>300</v>
       </c>
-      <c r="D4" s="3">
-        <f>SUM(Compras!F5,Compras!F13,Compras!F21)</f>
+      <c r="D4" s="2">
+        <f>SUM('Materia Prima'!F5,'Materia Prima'!F13,'Materia Prima'!F21)</f>
         <v>110</v>
       </c>
-      <c r="E4" s="3">
-        <f>SUM(Compras!F6,Compras!F14,Compras!F22)</f>
+      <c r="E4" s="2">
+        <f>SUM('Materia Prima'!F6,'Materia Prima'!F14,'Materia Prima'!F22)</f>
         <v>180</v>
       </c>
-      <c r="F4" s="3">
-        <f>SUM(Compras!F7,Compras!F15,Compras!F23)</f>
+      <c r="F4" s="2">
+        <f>SUM('Materia Prima'!F7,'Materia Prima'!F15,'Materia Prima'!F23)</f>
         <v>390</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="C1:F2"/>
     <mergeCell ref="G1:J2"/>
     <mergeCell ref="G3:J4"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="K3:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>